<commit_message>
personality and race-IAT study: Processing code -->Combine, Save to disk and master exclude variable
Combine the demographics, BFI, and IAT data into one data frame. This data frame should be one-row-one-participant. Both the mean scored and item level BFI data should be present in the dataset.
Create a master exclude variable from the individual exclude variables.
Save the processed data to the data/processed/ folder as “data_processed.csv”.
Create a codebook for the processed data file that explains what each variable represents.
</commit_message>
<xml_diff>
--- a/personality and race-IAT study/code/R_processing_codebook.xlsx
+++ b/personality and race-IAT study/code/R_processing_codebook.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -185,6 +185,9 @@
     <t xml:space="preserve">result_iat_perf</t>
   </si>
   <si>
+    <t xml:space="preserve">result_master_exclusion</t>
+  </si>
+  <si>
     <t xml:space="preserve">result_range_a</t>
   </si>
   <si>
@@ -248,10 +251,61 @@
     <t xml:space="preserve">Participant age</t>
   </si>
   <si>
+    <t xml:space="preserve">bfi_a_mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_c_mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_e_mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_n_mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bfi_o_mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude_bfi_completeness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude_bfi_logical_scores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude_iat_completeness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude_iat_performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude_participant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude_participant_without_bfi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude_participant_without_iat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude_unique_id_is.na</t>
+  </si>
+  <si>
     <t xml:space="preserve">gender</t>
   </si>
   <si>
     <t xml:space="preserve">Participant gender</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iat_D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iat_mean1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iat_mean2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iat_SD</t>
   </si>
   <si>
     <t xml:space="preserve">unique_id</t>
@@ -1376,7 +1430,7 @@
         <v>63</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
         <v>7</v>
@@ -1387,10 +1441,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
+        <v>64</v>
+      </c>
+      <c r="B54" t="s">
         <v>65</v>
-      </c>
-      <c r="B54" t="s">
-        <v>66</v>
       </c>
       <c r="C54" t="s">
         <v>7</v>
@@ -1401,10 +1455,10 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
+        <v>66</v>
+      </c>
+      <c r="B55" t="s">
         <v>67</v>
-      </c>
-      <c r="B55" t="s">
-        <v>68</v>
       </c>
       <c r="C55" t="s">
         <v>7</v>
@@ -1415,10 +1469,10 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>68</v>
+      </c>
+      <c r="B56" t="s">
         <v>69</v>
-      </c>
-      <c r="B56" t="s">
-        <v>7</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
@@ -1432,7 +1486,7 @@
         <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="C57" t="s">
         <v>7</v>
@@ -1443,11 +1497,17 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" t="s">
         <v>72</v>
       </c>
-      <c r="B58"/>
-      <c r="C58"/>
-      <c r="D58"/>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
@@ -1461,22 +1521,16 @@
       <c r="A60" t="s">
         <v>74</v>
       </c>
-      <c r="B60" t="s">
-        <v>75</v>
-      </c>
-      <c r="C60" t="s">
-        <v>7</v>
-      </c>
-      <c r="D60" t="s">
-        <v>7</v>
-      </c>
+      <c r="B60"/>
+      <c r="C60"/>
+      <c r="D60"/>
     </row>
     <row r="61">
       <c r="A61" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" t="s">
         <v>76</v>
-      </c>
-      <c r="B61" t="s">
-        <v>77</v>
       </c>
       <c r="C61" t="s">
         <v>7</v>
@@ -1487,10 +1541,10 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62" t="s">
         <v>78</v>
-      </c>
-      <c r="B62" t="s">
-        <v>79</v>
       </c>
       <c r="C62" t="s">
         <v>7</v>
@@ -1501,10 +1555,10 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B63" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="C63" t="s">
         <v>7</v>
@@ -1515,10 +1569,10 @@
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B64" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="C64" t="s">
         <v>7</v>
@@ -1529,10 +1583,10 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B65" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="C65" t="s">
         <v>7</v>
@@ -1543,10 +1597,10 @@
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B66" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="C66" t="s">
         <v>7</v>
@@ -1557,10 +1611,10 @@
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="C67" t="s">
         <v>7</v>
@@ -1571,10 +1625,10 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="C68" t="s">
         <v>7</v>
@@ -1585,10 +1639,10 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B69" t="s">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="C69" t="s">
         <v>7</v>
@@ -1599,10 +1653,10 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B70" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="C70" t="s">
         <v>7</v>
@@ -1613,10 +1667,10 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B71" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="C71" t="s">
         <v>7</v>
@@ -1627,10 +1681,10 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B72" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="C72" t="s">
         <v>7</v>
@@ -1641,15 +1695,249 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
+        <v>89</v>
+      </c>
+      <c r="B73"/>
+      <c r="C73"/>
+      <c r="D73"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>90</v>
+      </c>
+      <c r="B74"/>
+      <c r="C74"/>
+      <c r="D74"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>91</v>
+      </c>
+      <c r="B75"/>
+      <c r="C75"/>
+      <c r="D75"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>92</v>
+      </c>
+      <c r="B76" t="s">
+        <v>93</v>
+      </c>
+      <c r="C76" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>94</v>
+      </c>
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s">
+        <v>7</v>
+      </c>
+      <c r="D77" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>95</v>
+      </c>
+      <c r="B78" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>96</v>
+      </c>
+      <c r="B79" t="s">
+        <v>7</v>
+      </c>
+      <c r="C79" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>97</v>
+      </c>
+      <c r="B80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>98</v>
+      </c>
+      <c r="B81" t="s">
+        <v>99</v>
+      </c>
+      <c r="C81" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
         <v>100</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B82" t="s">
         <v>101</v>
       </c>
-      <c r="C73" t="s">
-        <v>7</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="C82" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>102</v>
+      </c>
+      <c r="B83" t="s">
+        <v>103</v>
+      </c>
+      <c r="C83" t="s">
+        <v>7</v>
+      </c>
+      <c r="D83" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>104</v>
+      </c>
+      <c r="B84" t="s">
+        <v>105</v>
+      </c>
+      <c r="C84" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>106</v>
+      </c>
+      <c r="B85" t="s">
+        <v>107</v>
+      </c>
+      <c r="C85" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>108</v>
+      </c>
+      <c r="B86" t="s">
+        <v>109</v>
+      </c>
+      <c r="C86" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>110</v>
+      </c>
+      <c r="B87" t="s">
+        <v>111</v>
+      </c>
+      <c r="C87" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>112</v>
+      </c>
+      <c r="B88" t="s">
+        <v>113</v>
+      </c>
+      <c r="C88" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>114</v>
+      </c>
+      <c r="B89" t="s">
+        <v>115</v>
+      </c>
+      <c r="C89" t="s">
+        <v>7</v>
+      </c>
+      <c r="D89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>116</v>
+      </c>
+      <c r="B90" t="s">
+        <v>117</v>
+      </c>
+      <c r="C90" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>118</v>
+      </c>
+      <c r="B91" t="s">
+        <v>119</v>
+      </c>
+      <c r="C91" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
personality and race-IAT study: update
mall improvements

calculation of mean value (not sum)
etc...
</commit_message>
<xml_diff>
--- a/personality and race-IAT study/code/R_processing_codebook.xlsx
+++ b/personality and race-IAT study/code/R_processing_codebook.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="112">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -128,34 +128,10 @@
     <t xml:space="preserve">All information for analysis without the master exclusion column and the three demographic exclusions</t>
   </si>
   <si>
-    <t xml:space="preserve">maxscore_bfi_a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maxscore_bfi_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maxscore_bfi_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maxscore_bfi_n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maxscore_bfi_o</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minscore_bfi_a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minscore_bfi_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minscore_bfi_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minscore_bfi_n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minscore_bfi_o</t>
+    <t xml:space="preserve">maxscore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minscore</t>
   </si>
   <si>
     <t xml:space="preserve">negative_values_a_exist</t>
@@ -1079,29 +1055,17 @@
       <c r="A28" t="s">
         <v>38</v>
       </c>
-      <c r="B28" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" t="s">
-        <v>7</v>
-      </c>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
     </row>
     <row r="29">
       <c r="A29" t="s">
         <v>39</v>
       </c>
-      <c r="B29" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
     </row>
     <row r="30">
       <c r="A30" t="s">
@@ -1332,7 +1296,7 @@
         <v>56</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
@@ -1343,10 +1307,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
@@ -1357,10 +1321,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -1371,7 +1335,7 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
@@ -1385,10 +1349,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -1399,38 +1363,26 @@
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>61</v>
-      </c>
-      <c r="B51" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" t="s">
-        <v>7</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>62</v>
-      </c>
-      <c r="B52" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" t="s">
-        <v>7</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="C53" t="s">
         <v>7</v>
@@ -1441,10 +1393,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B54" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C54" t="s">
         <v>7</v>
@@ -1455,10 +1407,10 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B55" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
         <v>7</v>
@@ -1469,10 +1421,10 @@
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B56" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
         <v>7</v>
@@ -1483,7 +1435,7 @@
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
@@ -1497,10 +1449,10 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B58" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="C58" t="s">
         <v>7</v>
@@ -1511,26 +1463,38 @@
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>73</v>
-      </c>
-      <c r="B59"/>
-      <c r="C59"/>
-      <c r="D59"/>
+        <v>75</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>74</v>
-      </c>
-      <c r="B60"/>
-      <c r="C60"/>
-      <c r="D60"/>
+        <v>76</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="C61" t="s">
         <v>7</v>
@@ -1541,10 +1505,10 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
         <v>7</v>
@@ -1585,50 +1549,32 @@
       <c r="A65" t="s">
         <v>81</v>
       </c>
-      <c r="B65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" t="s">
-        <v>7</v>
-      </c>
-      <c r="D65" t="s">
-        <v>7</v>
-      </c>
+      <c r="B65"/>
+      <c r="C65"/>
+      <c r="D65"/>
     </row>
     <row r="66">
       <c r="A66" t="s">
         <v>82</v>
       </c>
-      <c r="B66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" t="s">
-        <v>7</v>
-      </c>
-      <c r="D66" t="s">
-        <v>7</v>
-      </c>
+      <c r="B66"/>
+      <c r="C66"/>
+      <c r="D66"/>
     </row>
     <row r="67">
       <c r="A67" t="s">
         <v>83</v>
       </c>
-      <c r="B67" t="s">
-        <v>7</v>
-      </c>
-      <c r="C67" t="s">
-        <v>7</v>
-      </c>
-      <c r="D67" t="s">
-        <v>7</v>
-      </c>
+      <c r="B67"/>
+      <c r="C67"/>
+      <c r="D67"/>
     </row>
     <row r="68">
       <c r="A68" t="s">
         <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C68" t="s">
         <v>7</v>
@@ -1639,7 +1585,7 @@
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B69" t="s">
         <v>7</v>
@@ -1653,7 +1599,7 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
@@ -1667,7 +1613,7 @@
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B71" t="s">
         <v>7</v>
@@ -1681,7 +1627,7 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B72" t="s">
         <v>7</v>
@@ -1695,34 +1641,52 @@
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>89</v>
-      </c>
-      <c r="B73"/>
-      <c r="C73"/>
-      <c r="D73"/>
+        <v>90</v>
+      </c>
+      <c r="B73" t="s">
+        <v>91</v>
+      </c>
+      <c r="C73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>90</v>
-      </c>
-      <c r="B74"/>
-      <c r="C74"/>
-      <c r="D74"/>
+        <v>92</v>
+      </c>
+      <c r="B74" t="s">
+        <v>93</v>
+      </c>
+      <c r="C74" t="s">
+        <v>7</v>
+      </c>
+      <c r="D74" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>91</v>
-      </c>
-      <c r="B75"/>
-      <c r="C75"/>
-      <c r="D75"/>
+        <v>94</v>
+      </c>
+      <c r="B75" t="s">
+        <v>95</v>
+      </c>
+      <c r="C75" t="s">
+        <v>7</v>
+      </c>
+      <c r="D75" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B76" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C76" t="s">
         <v>7</v>
@@ -1733,10 +1697,10 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="C77" t="s">
         <v>7</v>
@@ -1747,10 +1711,10 @@
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B78" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="C78" t="s">
         <v>7</v>
@@ -1761,10 +1725,10 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B79" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="C79" t="s">
         <v>7</v>
@@ -1775,10 +1739,10 @@
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B80" t="s">
-        <v>7</v>
+        <v>105</v>
       </c>
       <c r="C80" t="s">
         <v>7</v>
@@ -1789,10 +1753,10 @@
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C81" t="s">
         <v>7</v>
@@ -1803,10 +1767,10 @@
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B82" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C82" t="s">
         <v>7</v>
@@ -1817,127 +1781,15 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="B83" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C83" t="s">
         <v>7</v>
       </c>
       <c r="D83" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
-        <v>104</v>
-      </c>
-      <c r="B84" t="s">
-        <v>105</v>
-      </c>
-      <c r="C84" t="s">
-        <v>7</v>
-      </c>
-      <c r="D84" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>106</v>
-      </c>
-      <c r="B85" t="s">
-        <v>107</v>
-      </c>
-      <c r="C85" t="s">
-        <v>7</v>
-      </c>
-      <c r="D85" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s">
-        <v>108</v>
-      </c>
-      <c r="B86" t="s">
-        <v>109</v>
-      </c>
-      <c r="C86" t="s">
-        <v>7</v>
-      </c>
-      <c r="D86" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s">
-        <v>110</v>
-      </c>
-      <c r="B87" t="s">
-        <v>111</v>
-      </c>
-      <c r="C87" t="s">
-        <v>7</v>
-      </c>
-      <c r="D87" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s">
-        <v>112</v>
-      </c>
-      <c r="B88" t="s">
-        <v>113</v>
-      </c>
-      <c r="C88" t="s">
-        <v>7</v>
-      </c>
-      <c r="D88" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s">
-        <v>114</v>
-      </c>
-      <c r="B89" t="s">
-        <v>115</v>
-      </c>
-      <c r="C89" t="s">
-        <v>7</v>
-      </c>
-      <c r="D89" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s">
-        <v>116</v>
-      </c>
-      <c r="B90" t="s">
-        <v>117</v>
-      </c>
-      <c r="C90" t="s">
-        <v>7</v>
-      </c>
-      <c r="D90" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s">
-        <v>118</v>
-      </c>
-      <c r="B91" t="s">
-        <v>119</v>
-      </c>
-      <c r="C91" t="s">
-        <v>7</v>
-      </c>
-      <c r="D91" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>